<commit_message>
fixed Alaina's test case, fixed FideliaAlsup, added test case for sanity
</commit_message>
<xml_diff>
--- a/tools/FHIRTestCases for VRDR IG validation and systems strengthening.xlsx
+++ b/tools/FHIRTestCases for VRDR IG validation and systems strengthening.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skravitz/git/vrdr-dotnet/tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5F0249-86B0-2243-820E-45AED198A9C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B7B7B30-5D1F-6942-8EF3-CA0FA7893353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="40040" windowHeight="21240" xr2:uid="{7A50F290-1C75-487E-9806-F93553E4E7CC}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="378">
   <si>
     <t>Pos</t>
   </si>
@@ -1973,8 +1973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35A3845B-6554-4658-A84C-1943C1210794}">
   <dimension ref="A1:I126"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="F74" sqref="F74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3901,8 +3901,8 @@
       <c r="E72" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="F72" s="11" t="s">
-        <v>60</v>
+      <c r="F72" s="11">
+        <v>2022</v>
       </c>
       <c r="G72" s="10" t="s">
         <v>19</v>
@@ -3928,7 +3928,7 @@
         <v>19</v>
       </c>
       <c r="F73" s="11">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="G73" s="10" t="s">
         <v>19</v>
@@ -3955,7 +3955,7 @@
         <v>19</v>
       </c>
       <c r="F74" s="11">
-        <v>2022</v>
+        <v>18</v>
       </c>
       <c r="G74" s="10" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
updates to test cases
</commit_message>
<xml_diff>
--- a/tools/FHIRTestCases for VRDR IG validation and systems strengthening.xlsx
+++ b/tools/FHIRTestCases for VRDR IG validation and systems strengthening.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skravitz/git/vrdr-dotnet/tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B7B7B30-5D1F-6942-8EF3-CA0FA7893353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{553032B3-B8B3-574E-AEA1-3C6FD2DD6DE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="40040" windowHeight="21240" xr2:uid="{7A50F290-1C75-487E-9806-F93553E4E7CC}"/>
   </bookViews>
@@ -1973,8 +1973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35A3845B-6554-4658-A84C-1943C1210794}">
   <dimension ref="A1:I126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="F74" sqref="F74"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
commit spreadsheet used to drive test case generation
</commit_message>
<xml_diff>
--- a/tools/FHIRTestCases for VRDR IG validation and systems strengthening.xlsx
+++ b/tools/FHIRTestCases for VRDR IG validation and systems strengthening.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skravitz/git/vrdr-dotnet/tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{553032B3-B8B3-574E-AEA1-3C6FD2DD6DE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{051C2A48-77DC-AD4C-87F3-229B539555B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="40040" windowHeight="21240" xr2:uid="{7A50F290-1C75-487E-9806-F93553E4E7CC}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="379">
   <si>
     <t>Pos</t>
   </si>
@@ -1516,6 +1516,22 @@
   </si>
   <si>
     <t>SSN</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CO 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Colorado)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1973,8 +1989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35A3845B-6554-4658-A84C-1943C1210794}">
   <dimension ref="A1:I126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="C70" sqref="C70"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="G72" sqref="G72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3876,7 +3892,7 @@
         <v>19</v>
       </c>
       <c r="G71" s="11" t="s">
-        <v>69</v>
+        <v>378</v>
       </c>
       <c r="H71" s="1" t="s">
         <v>372</v>
@@ -5372,15 +5388,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -5430,7 +5437,28 @@
 </spe:Receivers>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="b541edd5-2552-480e-ada6-0e2c8d317108">YVWEJ5DVYS2U-1209380688-131</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="b541edd5-2552-480e-ada6-0e2c8d317108">
+      <Url>https://cdcpartners.sharepoint.com/sites/NCHS/vrsd/_layouts/15/DocIdRedir.aspx?ID=YVWEJ5DVYS2U-1209380688-131</Url>
+      <Description>YVWEJ5DVYS2U-1209380688-131</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010015A1A77487579F48ABE6BEDF0427BAAC" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e10cea9757bc13a70f8c111e7d761854">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b541edd5-2552-480e-ada6-0e2c8d317108" xmlns:ns3="1bdcd305-59e3-4647-826e-69eceb9c0460" xmlns:ns4="7bbef1ec-d63f-46cc-930f-49c09922ffd3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2cb4dfd19fa2e8e9298fb72b1f5cfd4d" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="b541edd5-2552-480e-ada6-0e2c8d317108"/>
@@ -5625,19 +5653,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="b541edd5-2552-480e-ada6-0e2c8d317108">YVWEJ5DVYS2U-1209380688-131</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="b541edd5-2552-480e-ada6-0e2c8d317108">
-      <Url>https://cdcpartners.sharepoint.com/sites/NCHS/vrsd/_layouts/15/DocIdRedir.aspx?ID=YVWEJ5DVYS2U-1209380688-131</Url>
-      <Description>YVWEJ5DVYS2U-1209380688-131</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF0D7A6D-D78F-4048-9348-0B4289842B11}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{448710E8-BE9E-4C9E-A40A-0AC1DAE48E99}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -5645,15 +5669,17 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF0D7A6D-D78F-4048-9348-0B4289842B11}">
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69E3EF86-6C9E-4C22-A476-13DA012C68C5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b541edd5-2552-480e-ada6-0e2c8d317108"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2A73C3B-1842-4CE1-B61D-F1A110A49985}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5671,14 +5697,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69E3EF86-6C9E-4C22-A476-13DA012C68C5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b541edd5-2552-480e-ada6-0e2c8d317108"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>